<commit_message>
fixed the excel first row ignore first row and can be used to leave headings
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,12 +22,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">UserName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
   <si>
     <t xml:space="preserve">admin@email.com</t>
   </si>
   <si>
     <t xml:space="preserve">admin@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobby</t>
   </si>
   <si>
     <t xml:space="preserve">Jack Jonson</t>
@@ -76,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +123,23 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,13 +149,20 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border diagonalUp="true" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="hair"/>
     </border>
   </borders>
   <cellStyleXfs count="20">
@@ -142,13 +190,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -344,15 +404,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.22"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -360,9 +424,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="admin@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="admin@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -379,65 +451,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="admin098@email.com"/>
-    <hyperlink ref="C1" r:id="rId2" display="Test@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="admin098@email.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="Test@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -463,32 +558,32 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sorted the bug in excel reading
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="RegisterUserData" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="AddPIMUserData" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -54,16 +53,16 @@
     <t xml:space="preserve">Hobby</t>
   </si>
   <si>
-    <t xml:space="preserve">Jack Jonson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin098@email.com</t>
+    <t xml:space="preserve">Joseph Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@56oiu@email.com</t>
   </si>
   <si>
     <t xml:space="preserve">Test@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation Testing</t>
+    <t xml:space="preserve">Java</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -75,22 +74,16 @@
     <t xml:space="preserve">Playing</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mjmartin</t>
+    <t xml:space="preserve">Joseph Dillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joseph123674@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading</t>
   </si>
 </sst>
 </file>
@@ -100,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,15 +124,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,20 +133,13 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border diagonalUp="true" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal style="hair"/>
     </border>
   </borders>
   <cellStyleXfs count="20">
@@ -190,8 +167,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,18 +182,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -406,29 +375,29 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -451,145 +420,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.95"/>
+  </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="admin098@email.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="Test@123"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H1" r:id="rId1" display="Test@123"/>
-    <hyperlink ref="I1" r:id="rId2" display="Test@123"/>
+    <hyperlink ref="C2" r:id="rId1" display="Test@123"/>
+    <hyperlink ref="C3" r:id="rId2" display="Test@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Implemented the Random class for String Values, left 2 values for TDD in Excel
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -38,52 +38,13 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
     <t xml:space="preserve">State</t>
   </si>
   <si>
-    <t xml:space="preserve">Hobby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph Jackson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test@56oiu@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Punjab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph Dillon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joseph123674@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reading</t>
+    <t xml:space="preserve">Darryal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goa</t>
   </si>
 </sst>
 </file>
@@ -420,92 +381,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.95"/>
-  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Test@123"/>
-    <hyperlink ref="C3" r:id="rId2" display="Test@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>